<commit_message>
bug ko viet data dc vao o C15
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -2,21 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView activeTab="0"/>
-  </bookViews>
   <sheets>
     <sheet state="hidden" name="C_Hằng" sheetId="1" r:id="rId4"/>
     <sheet state="hidden" name=" Gỗ Veener" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Song lập" sheetId="3" r:id="rId6"/>
     <sheet state="hidden" name="Chỉ tủ bếp dưới" sheetId="4" r:id="rId7"/>
   </sheets>
+  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="142">
   <si>
     <t>A ONE</t>
   </si>
@@ -1444,103 +1442,6 @@
  - Đơn giá trên chưa bao gồm VAT, khách hàng chỉ chịu phí VAT = 10% tổng gía trị hợp đồng khi muốn xuất hóa đơn đỏ.
  - Bảo hành phần gỗ 3 năm, phụ kiện bảo hành 2 năm theo hãng.
  - Khối lượng thực tế tính theo kích thước tại công trình.</t>
-  </si>
-  <si>
-    <t>Modern</t>
-  </si>
-  <si>
-    <t>Khách hàng : long</t>
-  </si>
-  <si>
-    <t>Điện thoại: 0123123123</t>
-  </si>
-  <si>
-    <t>Địa chỉ: ha noi</t>
-  </si>
-  <si>
-    <t>Ngày: 02/08/2023</t>
-  </si>
-  <si>
-    <t>UserSelection(phongCachNoiThat=PhongCachNoiThat{id=1, name='Modern', noiThatList=[NoiThat(id=1, name=Table, hangMucList=[HangMuc(id=1, name=IndoorTable, vatLieuList=[VatLieu(id=1, name=Wood, thongSo=ThongSo(id=1, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=2, name=Metal, thongSo=ThongSo(id=2, dai=8, rong=6, cao=4, don_vi=cm, don_gia=45)), VatLieu(id=3, name=Plastic, thongSo=ThongSo(id=3, dai=12, rong=7, cao=2, don_vi=cm, don_gia=55))]), HangMuc(id=2, name=IndoorChair, vatLieuList=[VatLieu(id=4, name=Wood, thongSo=ThongSo(id=4, dai=15, rong=5, cao=3, don_vi=cm, don_gia=60)), VatLieu(id=5, name=Metal, thongSo=ThongSo(id=5, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=6, name=Plastic, thongSo=ThongSo(id=6, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50))])]), NoiThat(id=2, name=Chair, hangMucList=[HangMuc(id=3, name=IndoorBed, vatLieuList=[VatLieu(id=7, name=Wood, thongSo=ThongSo(id=7, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=8, name=Metal, thongSo=ThongSo(id=8, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=9, name=Plastic, thongSo=ThongSo(id=9, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50))])])]}, noiThat=NoiThat(id=1, name=Table, hangMucList=[HangMuc(id=1, name=IndoorTable, vatLieuList=[VatLieu(id=1, name=Wood, thongSo=ThongSo(id=1, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=2, name=Metal, thongSo=ThongSo(id=2, dai=8, rong=6, cao=4, don_vi=cm, don_gia=45)), VatLieu(id=3, name=Plastic, thongSo=ThongSo(id=3, dai=12, rong=7, cao=2, don_vi=cm, don_gia=55))]), HangMuc(id=2, name=IndoorChair, vatLieuList=[VatLieu(id=4, name=Wood, thongSo=ThongSo(id=4, dai=15, rong=5, cao=3, don_vi=cm, don_gia=60)), VatLieu(id=5, name=Metal, thongSo=ThongSo(id=5, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=6, name=Plastic, thongSo=ThongSo(id=6, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50))])]), hangMuc=HangMuc(id=1, name=IndoorTable, vatLieuList=[VatLieu(id=1, name=Wood, thongSo=ThongSo(id=1, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=2, name=Metal, thongSo=ThongSo(id=2, dai=8, rong=6, cao=4, don_vi=cm, don_gia=45)), VatLieu(id=3, name=Plastic, thongSo=ThongSo(id=3, dai=12, rong=7, cao=2, don_vi=cm, don_gia=55))]), vatLieu=VatLieu(id=1, name=Wood, thongSo=ThongSo(id=1, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), thongSo=ThongSo(id=1, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50))</t>
-  </si>
-  <si>
-    <t>UserSelection(phongCachNoiThat=PhongCachNoiThat{id=1, name='Modern', noiThatList=[NoiThat(id=1, name=Table, hangMucList=[HangMuc(id=1, name=IndoorTable, vatLieuList=[VatLieu(id=1, name=Wood, thongSo=ThongSo(id=1, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=2, name=Metal, thongSo=ThongSo(id=2, dai=8, rong=6, cao=4, don_vi=cm, don_gia=45)), VatLieu(id=3, name=Plastic, thongSo=ThongSo(id=3, dai=12, rong=7, cao=2, don_vi=cm, don_gia=55))]), HangMuc(id=2, name=IndoorChair, vatLieuList=[VatLieu(id=4, name=Wood, thongSo=ThongSo(id=4, dai=15, rong=5, cao=3, don_vi=cm, don_gia=60)), VatLieu(id=5, name=Metal, thongSo=ThongSo(id=5, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=6, name=Plastic, thongSo=ThongSo(id=6, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50))])]), NoiThat(id=2, name=Chair, hangMucList=[HangMuc(id=3, name=IndoorBed, vatLieuList=[VatLieu(id=7, name=Wood, thongSo=ThongSo(id=7, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=8, name=Metal, thongSo=ThongSo(id=8, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=9, name=Plastic, thongSo=ThongSo(id=9, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50))])])]}, noiThat=NoiThat(id=2, name=Chair, hangMucList=[HangMuc(id=3, name=IndoorBed, vatLieuList=[VatLieu(id=7, name=Wood, thongSo=ThongSo(id=7, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=8, name=Metal, thongSo=ThongSo(id=8, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=9, name=Plastic, thongSo=ThongSo(id=9, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50))])]), hangMuc=HangMuc(id=2, name=IndoorChair, vatLieuList=[VatLieu(id=4, name=Wood, thongSo=ThongSo(id=4, dai=15, rong=5, cao=3, don_vi=cm, don_gia=60)), VatLieu(id=5, name=Metal, thongSo=ThongSo(id=5, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50)), VatLieu(id=6, name=Plastic, thongSo=ThongSo(id=6, dai=10, rong=5, cao=3, don_vi=cm, don_gia=50))]), vatLieu=VatLieu(id=2, name=Metal, thongSo=ThongSo(id=2, dai=8, rong=6, cao=4, don_vi=cm, don_gia=45)), thongSo=ThongSo(id=2, dai=8, rong=6, cao=4, don_vi=cm, don_gia=45))</t>
-  </si>
-  <si>
-    <t>EMP ID</t>
-  </si>
-  <si>
-    <t>EMP NAME</t>
-  </si>
-  <si>
-    <t>DESIGNATION</t>
-  </si>
-  <si>
-    <t>Tủ bếp long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Thùng  : MDF chống ẩm an cường , độ dày 18mm </t>
-  </si>
-  <si>
-    <t>189</t>
-  </si>
-  <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>750</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,360,000
-</t>
-  </si>
-  <si>
-    <t>Tủ bếp linh</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>450</t>
-  </si>
-  <si>
-    <t>850</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,360,000
-</t>
-  </si>
-  <si>
-    <t>Tủ bếp linh1</t>
-  </si>
-  <si>
-    <t>Tủ bếp linh2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.00
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.00
-</t>
-  </si>
-  <si>
-    <t>2,360,000</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 29,055,000</t>
-  </si>
-  <si>
-    <t>3,360,000</t>
-  </si>
-  <si>
-    <t>2.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 30,055,000</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1452,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="93">
+  <fonts count="35">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1746,282 +1647,6 @@
       <color theme="1"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -2085,7 +1710,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="20">
     <border/>
     <border>
       <left style="thin">
@@ -2244,30 +1869,12 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="156">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2714,166 +2321,6 @@
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="23" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3097,21 +2544,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.57"/>
-    <col min="2" max="2" customWidth="true" width="24.43"/>
-    <col min="3" max="3" customWidth="true" width="50.14"/>
-    <col min="4" max="6" customWidth="true" width="11.43"/>
-    <col min="7" max="7" customWidth="true" width="13.86"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="12.86"/>
-    <col min="10" max="10" customWidth="true" width="20.0"/>
-    <col min="11" max="11" customWidth="true" hidden="true" width="37.14"/>
+    <col customWidth="1" min="1" max="1" width="11.57"/>
+    <col customWidth="1" min="2" max="2" width="24.43"/>
+    <col customWidth="1" min="3" max="3" width="50.14"/>
+    <col customWidth="1" min="4" max="6" width="11.43"/>
+    <col customWidth="1" min="7" max="7" width="13.86"/>
+    <col customWidth="1" min="8" max="8" width="20.0"/>
+    <col customWidth="1" min="9" max="9" width="12.86"/>
+    <col customWidth="1" min="10" max="10" width="20.0"/>
+    <col customWidth="1" hidden="1" min="11" max="11" width="37.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3207,24 +2653,61 @@
       <c r="K6" s="18"/>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="223">
-        <v>143</v>
-      </c>
+      <c r="A7" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="223">
-        <v>144</v>
-      </c>
+      <c r="A8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="223">
-        <v>145</v>
-      </c>
+      <c r="A9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="223">
-        <v>146</v>
-      </c>
+      <c r="A10" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
@@ -3290,88 +2773,95 @@
       <c r="J13" s="32"/>
     </row>
     <row r="14">
-      <c r="B14" t="s" s="220">
-        <v>142</v>
-      </c>
-      <c r="C14" t="s" s="220">
-        <v>142</v>
-      </c>
-      <c r="D14" t="s" s="220">
-        <v>142</v>
-      </c>
-      <c r="E14" t="s" s="220">
-        <v>142</v>
-      </c>
-      <c r="F14" t="s" s="220">
-        <v>142</v>
-      </c>
-      <c r="G14" t="s" s="220">
-        <v>142</v>
-      </c>
-      <c r="H14" t="s" s="220">
-        <v>142</v>
-      </c>
-      <c r="I14" t="s" s="220">
-        <v>142</v>
-      </c>
+      <c r="A14" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="37">
+        <f>SUM(J15:J19)</f>
+        <v>37896230</v>
+      </c>
+      <c r="K14" s="38"/>
     </row>
     <row r="15">
-      <c r="B15" t="s" s="222">
-        <v>152</v>
-      </c>
-      <c r="C15" t="s" s="222">
-        <v>153</v>
-      </c>
-      <c r="D15" t="s" s="222">
-        <v>154</v>
-      </c>
-      <c r="E15" t="s" s="222">
-        <v>155</v>
-      </c>
-      <c r="F15" t="s" s="222">
-        <v>156</v>
-      </c>
-      <c r="G15" t="s" s="222">
+      <c r="A15" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="39">
+        <f>2880+2819-600-800</f>
+        <v>4299</v>
+      </c>
+      <c r="E15" s="40">
+        <v>600.0</v>
+      </c>
+      <c r="F15" s="39">
+        <v>810.0</v>
+      </c>
+      <c r="G15" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="H15" t="s" s="222">
-        <v>167</v>
-      </c>
-      <c r="I15" t="s" s="222">
-        <v>168</v>
-      </c>
-      <c r="J15" t="s" s="222">
-        <v>169</v>
-      </c>
+      <c r="H15" s="43">
+        <v>3250000.0</v>
+      </c>
+      <c r="I15" s="44">
+        <f t="shared" ref="I15:I18" si="1">D15/10^3</f>
+        <v>4.299</v>
+      </c>
+      <c r="J15" s="45">
+        <f t="shared" ref="J15:J19" si="2">I15*H15</f>
+        <v>13971750</v>
+      </c>
+      <c r="K15" s="46"/>
     </row>
     <row r="16">
-      <c r="B16" t="s" s="222">
-        <v>164</v>
-      </c>
-      <c r="C16" t="s" s="222">
-        <v>153</v>
-      </c>
-      <c r="D16" t="s" s="222">
-        <v>159</v>
-      </c>
-      <c r="E16" t="s" s="222">
-        <v>160</v>
-      </c>
-      <c r="F16" t="s" s="222">
-        <v>161</v>
-      </c>
-      <c r="G16" t="s" s="222">
+      <c r="A16" s="39">
+        <v>2.0</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="39">
+        <v>2880.0</v>
+      </c>
+      <c r="E16" s="40">
+        <v>350.0</v>
+      </c>
+      <c r="F16" s="39">
+        <v>750.0</v>
+      </c>
+      <c r="G16" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="H16" t="s" s="222">
-        <v>170</v>
-      </c>
-      <c r="I16" t="s" s="222">
-        <v>171</v>
-      </c>
-      <c r="J16" t="s" s="222">
-        <v>172</v>
-      </c>
+      <c r="H16" s="43">
+        <v>2360000.0</v>
+      </c>
+      <c r="I16" s="44">
+        <f t="shared" si="1"/>
+        <v>2.88</v>
+      </c>
+      <c r="J16" s="45">
+        <f t="shared" si="2"/>
+        <v>6796800</v>
+      </c>
+      <c r="K16" s="46"/>
     </row>
     <row r="17">
       <c r="A17" s="39">
@@ -4036,21 +3526,20 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.57"/>
-    <col min="2" max="2" customWidth="true" width="24.43"/>
-    <col min="3" max="3" customWidth="true" width="50.14"/>
-    <col min="4" max="6" customWidth="true" width="11.43"/>
-    <col min="7" max="7" customWidth="true" width="13.86"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="12.86"/>
-    <col min="10" max="10" customWidth="true" width="20.0"/>
-    <col min="11" max="11" customWidth="true" hidden="true" width="37.14"/>
+    <col customWidth="1" min="1" max="1" width="11.57"/>
+    <col customWidth="1" min="2" max="2" width="24.43"/>
+    <col customWidth="1" min="3" max="3" width="50.14"/>
+    <col customWidth="1" min="4" max="6" width="11.43"/>
+    <col customWidth="1" min="7" max="7" width="13.86"/>
+    <col customWidth="1" min="8" max="8" width="20.0"/>
+    <col customWidth="1" min="9" max="9" width="12.86"/>
+    <col customWidth="1" min="10" max="10" width="20.0"/>
+    <col customWidth="1" hidden="1" min="11" max="11" width="37.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4966,21 +4455,20 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.57"/>
-    <col min="2" max="2" customWidth="true" width="24.43"/>
-    <col min="3" max="3" customWidth="true" width="42.57"/>
-    <col min="4" max="6" customWidth="true" width="11.43"/>
-    <col min="7" max="7" customWidth="true" width="13.86"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="12.86"/>
-    <col min="10" max="10" customWidth="true" width="20.0"/>
-    <col min="11" max="11" customWidth="true" hidden="true" width="37.14"/>
+    <col customWidth="1" min="1" max="1" width="11.57"/>
+    <col customWidth="1" min="2" max="2" width="24.43"/>
+    <col customWidth="1" min="3" max="3" width="42.57"/>
+    <col customWidth="1" min="4" max="6" width="11.43"/>
+    <col customWidth="1" min="7" max="7" width="13.86"/>
+    <col customWidth="1" min="8" max="8" width="20.0"/>
+    <col customWidth="1" min="9" max="9" width="12.86"/>
+    <col customWidth="1" min="10" max="10" width="20.0"/>
+    <col customWidth="1" hidden="1" min="11" max="11" width="37.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5783,22 +5271,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.86"/>
-    <col min="2" max="2" customWidth="true" width="22.29"/>
-    <col min="3" max="3" customWidth="true" width="50.14"/>
-    <col min="4" max="4" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="9.86"/>
-    <col min="6" max="6" customWidth="true" width="10.14"/>
-    <col min="7" max="7" customWidth="true" width="13.86"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="12.86"/>
-    <col min="10" max="10" customWidth="true" width="20.0"/>
+    <col customWidth="1" min="1" max="1" width="12.86"/>
+    <col customWidth="1" min="2" max="2" width="22.29"/>
+    <col customWidth="1" min="3" max="3" width="50.14"/>
+    <col customWidth="1" min="4" max="4" width="10.0"/>
+    <col customWidth="1" min="5" max="5" width="9.86"/>
+    <col customWidth="1" min="6" max="6" width="10.14"/>
+    <col customWidth="1" min="7" max="7" width="13.86"/>
+    <col customWidth="1" min="8" max="8" width="20.0"/>
+    <col customWidth="1" min="9" max="9" width="12.86"/>
+    <col customWidth="1" min="10" max="10" width="20.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="33.0" customHeight="1">

</xml_diff>

<commit_message>
add alot of feature
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -2,19 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="hidden" name="C_Hằng" sheetId="1" r:id="rId4"/>
     <sheet state="hidden" name=" Gỗ Veener" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Song lập" sheetId="3" r:id="rId6"/>
     <sheet state="hidden" name="Chỉ tủ bếp dưới" sheetId="4" r:id="rId7"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="148">
   <si>
     <t>A ONE</t>
   </si>
@@ -1442,6 +1444,24 @@
  - Đơn giá trên chưa bao gồm VAT, khách hàng chỉ chịu phí VAT = 10% tổng gía trị hợp đồng khi muốn xuất hóa đơn đỏ.
  - Bảo hành phần gỗ 3 năm, phụ kiện bảo hành 2 năm theo hãng.
  - Khối lượng thực tế tính theo kích thước tại công trình.</t>
+  </si>
+  <si>
+    <t>Khách hàng : long</t>
+  </si>
+  <si>
+    <t>Điện thoại: 0123123123</t>
+  </si>
+  <si>
+    <t>Địa chỉ: ha noi</t>
+  </si>
+  <si>
+    <t>Ngày: 04/08/2023</t>
+  </si>
+  <si>
+    <t>Khách hàng : huy</t>
+  </si>
+  <si>
+    <t>Địa chỉ: hasadasd sadas</t>
   </si>
 </sst>
 </file>
@@ -1452,7 +1472,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="38">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1647,6 +1667,21 @@
       <color theme="1"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1874,7 +1909,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="159">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2321,6 +2356,9 @@
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2544,20 +2582,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.57"/>
-    <col customWidth="1" min="2" max="2" width="24.43"/>
-    <col customWidth="1" min="3" max="3" width="50.14"/>
-    <col customWidth="1" min="4" max="6" width="11.43"/>
-    <col customWidth="1" min="7" max="7" width="13.86"/>
-    <col customWidth="1" min="8" max="8" width="20.0"/>
-    <col customWidth="1" min="9" max="9" width="12.86"/>
-    <col customWidth="1" min="10" max="10" width="20.0"/>
-    <col customWidth="1" hidden="1" min="11" max="11" width="37.14"/>
+    <col min="1" max="1" customWidth="true" width="11.57"/>
+    <col min="2" max="2" customWidth="true" width="24.43"/>
+    <col min="3" max="3" customWidth="true" width="50.14"/>
+    <col min="4" max="6" customWidth="true" width="11.43"/>
+    <col min="7" max="7" customWidth="true" width="13.86"/>
+    <col min="8" max="8" customWidth="true" width="20.0"/>
+    <col min="9" max="9" customWidth="true" width="12.86"/>
+    <col min="10" max="10" customWidth="true" width="20.0"/>
+    <col min="11" max="11" customWidth="true" hidden="true" width="37.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2653,61 +2692,24 @@
       <c r="K6" s="18"/>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="20"/>
+      <c r="A7" t="s" s="158">
+        <v>146</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="20"/>
+      <c r="A8" t="s" s="158">
+        <v>143</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
+      <c r="A9" t="s" s="158">
+        <v>147</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="20"/>
+      <c r="A10" t="s" s="158">
+        <v>145</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
@@ -3526,20 +3528,21 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.57"/>
-    <col customWidth="1" min="2" max="2" width="24.43"/>
-    <col customWidth="1" min="3" max="3" width="50.14"/>
-    <col customWidth="1" min="4" max="6" width="11.43"/>
-    <col customWidth="1" min="7" max="7" width="13.86"/>
-    <col customWidth="1" min="8" max="8" width="20.0"/>
-    <col customWidth="1" min="9" max="9" width="12.86"/>
-    <col customWidth="1" min="10" max="10" width="20.0"/>
-    <col customWidth="1" hidden="1" min="11" max="11" width="37.14"/>
+    <col min="1" max="1" customWidth="true" width="11.57"/>
+    <col min="2" max="2" customWidth="true" width="24.43"/>
+    <col min="3" max="3" customWidth="true" width="50.14"/>
+    <col min="4" max="6" customWidth="true" width="11.43"/>
+    <col min="7" max="7" customWidth="true" width="13.86"/>
+    <col min="8" max="8" customWidth="true" width="20.0"/>
+    <col min="9" max="9" customWidth="true" width="12.86"/>
+    <col min="10" max="10" customWidth="true" width="20.0"/>
+    <col min="11" max="11" customWidth="true" hidden="true" width="37.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4455,20 +4458,21 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.57"/>
-    <col customWidth="1" min="2" max="2" width="24.43"/>
-    <col customWidth="1" min="3" max="3" width="42.57"/>
-    <col customWidth="1" min="4" max="6" width="11.43"/>
-    <col customWidth="1" min="7" max="7" width="13.86"/>
-    <col customWidth="1" min="8" max="8" width="20.0"/>
-    <col customWidth="1" min="9" max="9" width="12.86"/>
-    <col customWidth="1" min="10" max="10" width="20.0"/>
-    <col customWidth="1" hidden="1" min="11" max="11" width="37.14"/>
+    <col min="1" max="1" customWidth="true" width="11.57"/>
+    <col min="2" max="2" customWidth="true" width="24.43"/>
+    <col min="3" max="3" customWidth="true" width="42.57"/>
+    <col min="4" max="6" customWidth="true" width="11.43"/>
+    <col min="7" max="7" customWidth="true" width="13.86"/>
+    <col min="8" max="8" customWidth="true" width="20.0"/>
+    <col min="9" max="9" customWidth="true" width="12.86"/>
+    <col min="10" max="10" customWidth="true" width="20.0"/>
+    <col min="11" max="11" customWidth="true" hidden="true" width="37.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5271,21 +5275,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.86"/>
-    <col customWidth="1" min="2" max="2" width="22.29"/>
-    <col customWidth="1" min="3" max="3" width="50.14"/>
-    <col customWidth="1" min="4" max="4" width="10.0"/>
-    <col customWidth="1" min="5" max="5" width="9.86"/>
-    <col customWidth="1" min="6" max="6" width="10.14"/>
-    <col customWidth="1" min="7" max="7" width="13.86"/>
-    <col customWidth="1" min="8" max="8" width="20.0"/>
-    <col customWidth="1" min="9" max="9" width="12.86"/>
-    <col customWidth="1" min="10" max="10" width="20.0"/>
+    <col min="1" max="1" customWidth="true" width="12.86"/>
+    <col min="2" max="2" customWidth="true" width="22.29"/>
+    <col min="3" max="3" customWidth="true" width="50.14"/>
+    <col min="4" max="4" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="9.86"/>
+    <col min="6" max="6" customWidth="true" width="10.14"/>
+    <col min="7" max="7" customWidth="true" width="13.86"/>
+    <col min="8" max="8" customWidth="true" width="20.0"/>
+    <col min="9" max="9" customWidth="true" width="12.86"/>
+    <col min="10" max="10" customWidth="true" width="20.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="33.0" customHeight="1">

</xml_diff>